<commit_message>
add function get_DF for money-market.
</commit_message>
<xml_diff>
--- a/SwapPricing/sample_moneymarket.xlsx
+++ b/SwapPricing/sample_moneymarket.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susynishida/Desktop/dev_python/Finance/SwapPricing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michinobu/Desktop/dev_python/Finance/SwapPricing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="480" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="create_cashflow" sheetId="1" r:id="rId1"/>
@@ -179,8 +179,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -189,10 +193,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -526,7 +534,7 @@
         <v>43094</v>
       </c>
       <c r="C4" s="1">
-        <f>B4+IF(E4=1, 360, 0)*LEFT(A4,1)+IF(F4=1, 30, 0)*LEFT(A4,1)+IF(G4=1, 7, 0)*LEFT(A4,1)</f>
+        <f>B4+IF(E4=1,360,0)*LEFT(A4,LEN(A4)-1)+IF(F4=1,30,0)*LEFT(A4,LEN(A4)-1)+IF(G4=1,7,0)*LEFT(A4,LEN(A4)-1)</f>
         <v>43101</v>
       </c>
       <c r="D4" t="str">
@@ -555,23 +563,23 @@
         <v>43094</v>
       </c>
       <c r="C5" s="1">
-        <f>B5+IF(E5=1, 360, 0)*LEFT(A5,1)+IF(F5=1, 30, 0)*LEFT(A5,1)+IF(G5=1, 7, 0)*LEFT(A5,1)</f>
+        <f t="shared" ref="C5:C9" si="1">B5+IF(E5=1,360,0)*LEFT(A5,LEN(A5)-1)+IF(F5=1,30,0)*LEFT(A5,LEN(A5)-1)+IF(G5=1,7,0)*LEFT(A5,LEN(A5)-1)</f>
         <v>43108</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D10" si="1">RIGHT(A5,1)</f>
+        <f t="shared" ref="D5:D10" si="2">RIGHT(A5,1)</f>
         <v>W</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E10" si="2">IF($D5="Y", 1, 0)</f>
+        <f t="shared" ref="E5:E10" si="3">IF($D5="Y", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F10" si="3">IF($D5="M", 1, 0)</f>
+        <f t="shared" ref="F5:F10" si="4">IF($D5="M", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G10" si="4">IF($D5="W", 1, 0)</f>
+        <f t="shared" ref="G5:G10" si="5">IF($D5="W", 1, 0)</f>
         <v>1</v>
       </c>
     </row>
@@ -584,15 +592,15 @@
         <v>43094</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C10" si="5">B6+IF(E6=1, 360, 0)*LEFT(A6,1)+IF(F6=1, 30, 0)*LEFT(A6,1)+IF(G6=1, 7, 0)*LEFT(A6,1)</f>
+        <f t="shared" si="1"/>
         <v>43124</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -600,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -613,23 +621,23 @@
         <v>43094</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>43154</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="5"/>
-        <v>43154</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="1"/>
-        <v>M</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -642,23 +650,23 @@
         <v>43094</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>43184</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="5"/>
-        <v>43184</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="1"/>
-        <v>M</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -671,23 +679,23 @@
         <v>43094</v>
       </c>
       <c r="C9" s="1">
+        <f t="shared" si="1"/>
+        <v>43274</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="5"/>
-        <v>43274</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="1"/>
-        <v>M</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -700,23 +708,23 @@
         <v>43094</v>
       </c>
       <c r="C10" s="1">
+        <f>B10+IF(E10=1,360,0)*LEFT(A10,LEN(A10)-1)+IF(F10=1,30,0)*LEFT(A10,LEN(A10)-1)+IF(G10=1,7,0)*LEFT(A10,LEN(A10)-1)</f>
+        <v>43454</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="5"/>
-        <v>43124</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="1"/>
-        <v>M</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -729,15 +737,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -748,7 +756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -759,10 +767,14 @@
         <v>43093</v>
       </c>
       <c r="D2" s="2">
-        <v>1.41E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4348E-2</v>
+      </c>
+      <c r="E2">
+        <f>1/(1+(C2-B2)/360*D2)</f>
+        <v>0.99996014603284633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -773,10 +785,14 @@
         <v>43094</v>
       </c>
       <c r="D3" s="2">
-        <v>1.41E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4348E-2</v>
+      </c>
+      <c r="E3">
+        <f>E2/(1+(C3-B3)/360*D3)</f>
+        <v>0.99992029365403134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -787,10 +803,14 @@
         <v>43101</v>
       </c>
       <c r="D4" s="2">
-        <v>1.91E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4876E-2</v>
+      </c>
+      <c r="E4">
+        <f>$E$3/(1+(C4-B4)/360*D4)</f>
+        <v>0.99963114479189386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -801,10 +821,14 @@
         <v>43108</v>
       </c>
       <c r="D5" s="2">
-        <v>2.0899999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E10" si="0">$E$3/(1+(C5-B5)/360*D5)</f>
+        <v>0.99933734686835807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -815,10 +839,14 @@
         <v>43124</v>
       </c>
       <c r="D6" s="2">
-        <v>2.49E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5630000000000002E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.99861959163592562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -829,10 +857,14 @@
         <v>43154</v>
       </c>
       <c r="D7" s="2">
-        <v>3.4499999999999999E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.6160000000000001E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.9972344089791807</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -843,10 +875,14 @@
         <v>43184</v>
       </c>
       <c r="D8" s="2">
-        <v>4.5700000000000003E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.685E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.99572579872689437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -857,10 +893,14 @@
         <v>43274</v>
       </c>
       <c r="D9" s="2">
-        <v>6.5399999999999998E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.8329999999999999E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.99083925191027356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -868,10 +908,14 @@
         <v>43094</v>
       </c>
       <c r="C10" s="1">
-        <v>43124</v>
+        <v>43454</v>
       </c>
       <c r="D10" s="2">
-        <v>9.1299999999999992E-3</v>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.97935386254067724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>